<commit_message>
Precision at k calculation
</commit_message>
<xml_diff>
--- a/LASCAD/results/similarApps/Experiments/Clusters/Graph/test.xlsx
+++ b/LASCAD/results/similarApps/Experiments/Clusters/Graph/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RaulMedeiros/Documents/19CustomDiff/LASCAD/LASCAD/results/similarApps/Experiments/Clusters/Graph/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886B494A-93FC-CB44-B754-A5474E165619}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C131A5-41A0-4C4E-8E64-78019E2425BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{99946AC7-C551-C04B-8FE7-7744F102796A}"/>
   </bookViews>
@@ -117,7 +117,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -132,6 +132,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,11 +167,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,7 +494,7 @@
   <dimension ref="A1:E218"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,7 +522,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3">
-        <v>2.69402037677742E+16</v>
+        <v>2.6940203767774298</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -518,8 +532,8 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3">
-        <v>2597680172628730</v>
+      <c r="C3" s="4">
+        <v>2.59768017262873</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -529,8 +543,8 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3">
-        <v>2469419696189080</v>
+      <c r="C4" s="4">
+        <v>2.46941969618908</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -540,8 +554,8 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3">
-        <v>2.38753242224356E+16</v>
+      <c r="C5" s="4">
+        <v>2.3875324222435599</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -551,8 +565,8 @@
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3">
-        <v>2.37778344190509E+16</v>
+      <c r="C6" s="4">
+        <v>2.3777834419050898</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -562,8 +576,8 @@
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3">
-        <v>2.05241388507763E+16</v>
+      <c r="C7" s="4">
+        <v>2.0524138850776299</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -573,8 +587,8 @@
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3">
-        <v>1771705453175350</v>
+      <c r="C8" s="4">
+        <v>1.77170545317535</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -584,8 +598,8 @@
       <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3">
-        <v>1.73205555486039E+16</v>
+      <c r="C9" s="4">
+        <v>1.73205555486039</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -595,8 +609,8 @@
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3">
-        <v>1685459762843120</v>
+      <c r="C10" s="4">
+        <v>1.68545976284312</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -606,8 +620,8 @@
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="3">
-        <v>1.68395329860972E+16</v>
+      <c r="C11" s="4">
+        <v>1.6839532986097201</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -617,8 +631,8 @@
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="3">
-        <v>1.68383991212513E+16</v>
+      <c r="C12" s="4">
+        <v>1.68383991212513</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -628,8 +642,8 @@
       <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="3">
-        <v>1682333750148240</v>
+      <c r="C13" s="4">
+        <v>1.68233375014824</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -639,8 +653,8 @@
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="3">
-        <v>1.68085413972208E+16</v>
+      <c r="C14" s="4">
+        <v>1.68085413972208</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -650,8 +664,8 @@
       <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="3">
-        <v>1678086821685300</v>
+      <c r="C15" s="4">
+        <v>1.6780868216853</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -661,8 +675,8 @@
       <c r="B16" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="3">
-        <v>2.95766267941654E+16</v>
+      <c r="C16" s="4">
+        <v>2.9576626794165399</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -672,8 +686,8 @@
       <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="3">
-        <v>2.861234948726E+16</v>
+      <c r="C17" s="4">
+        <v>2.861234948726</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -683,8 +697,8 @@
       <c r="B18" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="3">
-        <v>2.38753242224356E+16</v>
+      <c r="C18" s="4">
+        <v>2.3875324222435599</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -694,8 +708,8 @@
       <c r="B19" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="3">
-        <v>1.85707166530735E+16</v>
+      <c r="C19" s="4">
+        <v>1.85707166530735</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -705,8 +719,8 @@
       <c r="B20" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="3">
-        <v>1.7181573049434E+16</v>
+      <c r="C20" s="4">
+        <v>1.7181573049434</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -716,8 +730,8 @@
       <c r="B21" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="3">
-        <v>1707418864496270</v>
+      <c r="C21" s="4">
+        <v>1.70741886449627</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -727,8 +741,8 @@
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="3">
-        <v>1.68536336389156E+16</v>
+      <c r="C22" s="4">
+        <v>1.6853633638915599</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -738,8 +752,8 @@
       <c r="B23" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="3">
-        <v>1684578689698250</v>
+      <c r="C23" s="4">
+        <v>1.68457868969825</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -749,8 +763,8 @@
       <c r="B24" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="3">
-        <v>1684139117582440</v>
+      <c r="C24" s="4">
+        <v>1.6841391175824401</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -760,8 +774,8 @@
       <c r="B25" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="3">
-        <v>1.68282084484417E+16</v>
+      <c r="C25" s="4">
+        <v>1.6828208448441699</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -771,8 +785,8 @@
       <c r="B26" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="3">
-        <v>1.68188892900813E+16</v>
+      <c r="C26" s="4">
+        <v>1.68188892900813</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -782,8 +796,8 @@
       <c r="B27" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="3">
-        <v>1.68143257660378E+16</v>
+      <c r="C27" s="4">
+        <v>1.6814325766037801</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -793,8 +807,8 @@
       <c r="B28" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="3">
-        <v>1681268440095830</v>
+      <c r="C28" s="4">
+        <v>1.68126844009583</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -804,8 +818,8 @@
       <c r="B29" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="3">
-        <v>1.68125952784681E+16</v>
+      <c r="C29" s="4">
+        <v>1.6812595278468101</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -815,8 +829,8 @@
       <c r="B30" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="3">
-        <v>1.68090986136195E+16</v>
+      <c r="C30" s="4">
+        <v>1.68090986136195</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -826,8 +840,8 @@
       <c r="B31" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="3">
-        <v>1.67878330761273E+16</v>
+      <c r="C31" s="4">
+        <v>1.6787833076127301</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -837,8 +851,8 @@
       <c r="B32" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="3">
-        <v>1678593679214080</v>
+      <c r="C32" s="4">
+        <v>1.6785936792140801</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -848,8 +862,8 @@
       <c r="B33" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="3">
-        <v>284846686700151</v>
+      <c r="C33" s="4">
+        <v>2.8484668670015099</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -859,8 +873,8 @@
       <c r="B34" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="3">
-        <v>269582667556796</v>
+      <c r="C34" s="4">
+        <v>2.6958266755679601</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -870,8 +884,8 @@
       <c r="B35" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="3">
-        <v>2681847389501600</v>
+      <c r="C35" s="4">
+        <v>2.6818473895016002</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -881,8 +895,8 @@
       <c r="B36" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="3">
-        <v>1.6842912289947E+16</v>
+      <c r="C36" s="4">
+        <v>1.6842912289947001</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -892,8 +906,8 @@
       <c r="B37" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="3">
-        <v>1.68089781568594E+16</v>
+      <c r="C37" s="4">
+        <v>1.68089781568594</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -903,8 +917,8 @@
       <c r="B38" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="3">
-        <v>1.67995675037302E+16</v>
+      <c r="C38" s="4">
+        <v>1.6799567503730199</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -914,8 +928,8 @@
       <c r="B39" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="3">
-        <v>1.67980988261053E+16</v>
+      <c r="C39" s="4">
+        <v>1.6798098826105301</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -925,8 +939,8 @@
       <c r="B40" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="3">
-        <v>1678593679214080</v>
+      <c r="C40" s="4">
+        <v>1.6785936792140801</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -936,8 +950,8 @@
       <c r="B41" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="3">
-        <v>1678086821685300</v>
+      <c r="C41" s="4">
+        <v>1.6780868216853</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -947,8 +961,8 @@
       <c r="B42" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="3">
-        <v>284846686700151</v>
+      <c r="C42" s="4">
+        <v>2.8484668670015099</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -958,8 +972,8 @@
       <c r="B43" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="3">
-        <v>2616308305850640</v>
+      <c r="C43" s="4">
+        <v>2.61630830585064</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -969,8 +983,8 @@
       <c r="B44" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="3">
-        <v>2484740990245300</v>
+      <c r="C44" s="4">
+        <v>2.4847409902452999</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -980,8 +994,8 @@
       <c r="B45" t="s">
         <v>3</v>
       </c>
-      <c r="C45" s="3">
-        <v>2.413547675853E+16</v>
+      <c r="C45" s="4">
+        <v>2.4135476758530001</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -991,8 +1005,8 @@
       <c r="B46" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="3">
-        <v>2.28910423902995E+16</v>
+      <c r="C46" s="4">
+        <v>2.2891042390299599</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1002,8 +1016,8 @@
       <c r="B47" t="s">
         <v>1</v>
       </c>
-      <c r="C47" s="3">
-        <v>2196599519739470</v>
+      <c r="C47" s="4">
+        <v>2.1965995197394701</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1013,8 +1027,8 @@
       <c r="B48" t="s">
         <v>2</v>
       </c>
-      <c r="C48" s="3">
-        <v>2.18817070475403E+16</v>
+      <c r="C48" s="4">
+        <v>2.1881707047540302</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1024,8 +1038,8 @@
       <c r="B49" t="s">
         <v>16</v>
       </c>
-      <c r="C49" s="3">
-        <v>214990619808504</v>
+      <c r="C49" s="4">
+        <v>2.1499061980850298</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1035,8 +1049,8 @@
       <c r="B50" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="3">
-        <v>2.01117868118711E+16</v>
+      <c r="C50" s="4">
+        <v>2.01117868118711</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1046,8 +1060,8 @@
       <c r="B51" t="s">
         <v>17</v>
       </c>
-      <c r="C51" s="3">
-        <v>2.00745135363793E+16</v>
+      <c r="C51" s="4">
+        <v>2.0074513536379301</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -1057,8 +1071,8 @@
       <c r="B52" t="s">
         <v>9</v>
       </c>
-      <c r="C52" s="3">
-        <v>1.69710485039184E+16</v>
+      <c r="C52" s="4">
+        <v>1.69710485039184</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1068,8 +1082,8 @@
       <c r="B53" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="3">
-        <v>1690448028272840</v>
+      <c r="C53" s="4">
+        <v>1.69044802827284</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -1079,8 +1093,8 @@
       <c r="B54" t="s">
         <v>18</v>
       </c>
-      <c r="C54" s="3">
-        <v>1.68835769146761E+16</v>
+      <c r="C54" s="4">
+        <v>1.6883576914676099</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1090,8 +1104,8 @@
       <c r="B55" t="s">
         <v>19</v>
       </c>
-      <c r="C55" s="3">
-        <v>1.68703327219465E+16</v>
+      <c r="C55" s="4">
+        <v>1.6870332721946499</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1101,8 +1115,8 @@
       <c r="B56" t="s">
         <v>4</v>
       </c>
-      <c r="C56" s="3">
-        <v>1684139117582440</v>
+      <c r="C56" s="4">
+        <v>1.6841391175824401</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1112,8 +1126,8 @@
       <c r="B57" t="s">
         <v>0</v>
       </c>
-      <c r="C57" s="3">
-        <v>1.68383991212513E+16</v>
+      <c r="C57" s="4">
+        <v>1.68383991212513</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1123,8 +1137,8 @@
       <c r="B58" t="s">
         <v>8</v>
       </c>
-      <c r="C58" s="3">
-        <v>2.74351073603988E+16</v>
+      <c r="C58" s="4">
+        <v>2.7435107360398798</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -1134,8 +1148,8 @@
       <c r="B59" t="s">
         <v>14</v>
       </c>
-      <c r="C59" s="3">
-        <v>2681847389501600</v>
+      <c r="C59" s="4">
+        <v>2.6818473895016002</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -1145,8 +1159,8 @@
       <c r="B60" t="s">
         <v>12</v>
       </c>
-      <c r="C60" s="3">
-        <v>2610361513052920</v>
+      <c r="C60" s="4">
+        <v>2.6103615130529199</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -1156,8 +1170,8 @@
       <c r="B61" t="s">
         <v>13</v>
       </c>
-      <c r="C61" s="3">
-        <v>2.58038902852308E+16</v>
+      <c r="C61" s="4">
+        <v>2.5803890285230802</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -1167,8 +1181,8 @@
       <c r="B62" t="s">
         <v>7</v>
       </c>
-      <c r="C62" s="3">
-        <v>2278737125761410</v>
+      <c r="C62" s="4">
+        <v>2.2787371257614102</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -1178,8 +1192,8 @@
       <c r="B63" t="s">
         <v>11</v>
       </c>
-      <c r="C63" s="3">
-        <v>2.00745135363793E+16</v>
+      <c r="C63" s="4">
+        <v>2.0074513536379301</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -1189,8 +1203,8 @@
       <c r="B64" t="s">
         <v>9</v>
       </c>
-      <c r="C64" s="3">
-        <v>1.69138384332405E+16</v>
+      <c r="C64" s="4">
+        <v>1.69138384332405</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -1200,8 +1214,8 @@
       <c r="B65" t="s">
         <v>5</v>
       </c>
-      <c r="C65" s="3">
-        <v>1685536223205350</v>
+      <c r="C65" s="4">
+        <v>1.6855362232053499</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -1211,8 +1225,8 @@
       <c r="B66" t="s">
         <v>4</v>
       </c>
-      <c r="C66" s="3">
-        <v>1681268440095830</v>
+      <c r="C66" s="4">
+        <v>1.68126844009583</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -1222,8 +1236,8 @@
       <c r="B67" t="s">
         <v>15</v>
       </c>
-      <c r="C67" s="3">
-        <v>260134299002341</v>
+      <c r="C67" s="4">
+        <v>2.6013429900234</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -1233,8 +1247,8 @@
       <c r="B68" t="s">
         <v>3</v>
       </c>
-      <c r="C68" s="3">
-        <v>2.44144993186361E+16</v>
+      <c r="C68" s="4">
+        <v>2.4414499318636098</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -1244,8 +1258,8 @@
       <c r="B69" t="s">
         <v>1</v>
       </c>
-      <c r="C69" s="3">
-        <v>2.29328205843498E+16</v>
+      <c r="C69" s="4">
+        <v>2.29328205843498</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -1255,8 +1269,8 @@
       <c r="B70" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="3">
-        <v>2.10500966253373E+16</v>
+      <c r="C70" s="4">
+        <v>2.10500966253373</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -1266,8 +1280,8 @@
       <c r="B71" t="s">
         <v>2</v>
       </c>
-      <c r="C71" s="3">
-        <v>2092557511608830</v>
+      <c r="C71" s="4">
+        <v>2.0925575116088302</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -1277,8 +1291,8 @@
       <c r="B72" t="s">
         <v>6</v>
       </c>
-      <c r="C72" s="3">
-        <v>2.0446997306715E+16</v>
+      <c r="C72" s="4">
+        <v>2.0446997306714998</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -1288,8 +1302,8 @@
       <c r="B73" t="s">
         <v>8</v>
       </c>
-      <c r="C73" s="3">
-        <v>1.74610355312812E+16</v>
+      <c r="C73" s="4">
+        <v>1.7461035531281199</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -1299,8 +1313,8 @@
       <c r="B74" t="s">
         <v>7</v>
       </c>
-      <c r="C74" s="3">
-        <v>1.69284761827952E+16</v>
+      <c r="C74" s="4">
+        <v>1.69284761827952</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -1310,8 +1324,8 @@
       <c r="B75" t="s">
         <v>10</v>
       </c>
-      <c r="C75" s="3">
-        <v>1.68902751445241E+16</v>
+      <c r="C75" s="4">
+        <v>1.6890275144524101</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -1321,8 +1335,8 @@
       <c r="B76" t="s">
         <v>11</v>
       </c>
-      <c r="C76" s="3">
-        <v>1.68835769146761E+16</v>
+      <c r="C76" s="4">
+        <v>1.6883576914676099</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -1332,8 +1346,8 @@
       <c r="B77" t="s">
         <v>12</v>
       </c>
-      <c r="C77" s="3">
-        <v>1.68625810616996E+16</v>
+      <c r="C77" s="4">
+        <v>1.68625810616996</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -1343,8 +1357,8 @@
       <c r="B78" t="s">
         <v>13</v>
       </c>
-      <c r="C78" s="3">
-        <v>1684107791431590</v>
+      <c r="C78" s="4">
+        <v>1.6841077914315901</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -1354,8 +1368,8 @@
       <c r="B79" t="s">
         <v>4</v>
       </c>
-      <c r="C79" s="3">
-        <v>1.68125952784681E+16</v>
+      <c r="C79" s="4">
+        <v>1.6812595278468101</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -1365,8 +1379,8 @@
       <c r="B80" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="3">
-        <v>1.67995675037302E+16</v>
+      <c r="C80" s="4">
+        <v>1.6799567503730199</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -1376,8 +1390,8 @@
       <c r="B81" t="s">
         <v>6</v>
       </c>
-      <c r="C81" s="3">
-        <v>2.62349025029971E+16</v>
+      <c r="C81" s="4">
+        <v>2.6234902502997102</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -1387,8 +1401,8 @@
       <c r="B82" t="s">
         <v>17</v>
       </c>
-      <c r="C82" s="3">
-        <v>2610361513052920</v>
+      <c r="C82" s="4">
+        <v>2.6103615130529199</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -1398,8 +1412,8 @@
       <c r="B83" t="s">
         <v>9</v>
       </c>
-      <c r="C83" s="3">
-        <v>1694104809233910</v>
+      <c r="C83" s="4">
+        <v>1.6941048092339099</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -1409,8 +1423,8 @@
       <c r="B84" t="s">
         <v>5</v>
       </c>
-      <c r="C84" s="3">
-        <v>1.6881049422915E+16</v>
+      <c r="C84" s="4">
+        <v>1.6881049422915</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -1420,8 +1434,8 @@
       <c r="B85" t="s">
         <v>18</v>
       </c>
-      <c r="C85" s="3">
-        <v>1.68625810616996E+16</v>
+      <c r="C85" s="4">
+        <v>1.68625810616996</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -1431,8 +1445,8 @@
       <c r="B86" t="s">
         <v>19</v>
       </c>
-      <c r="C86" s="3">
-        <v>1685344442868060</v>
+      <c r="C86" s="4">
+        <v>1.68534444286806</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -1442,8 +1456,8 @@
       <c r="B87" t="s">
         <v>4</v>
       </c>
-      <c r="C87" s="3">
-        <v>1.68282084484417E+16</v>
+      <c r="C87" s="4">
+        <v>1.6828208448441699</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -1453,8 +1467,8 @@
       <c r="B88" t="s">
         <v>0</v>
       </c>
-      <c r="C88" s="3">
-        <v>1682333750148240</v>
+      <c r="C88" s="4">
+        <v>1.68233375014824</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -1464,8 +1478,8 @@
       <c r="B89" t="s">
         <v>5</v>
       </c>
-      <c r="C89" s="3">
-        <v>2.43021571881643E+16</v>
+      <c r="C89" s="4">
+        <v>2.4302157188164299</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -1475,8 +1489,8 @@
       <c r="B90" t="s">
         <v>8</v>
       </c>
-      <c r="C90" s="3">
-        <v>1.75580608424507E+16</v>
+      <c r="C90" s="4">
+        <v>1.75580608424507</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -1486,8 +1500,8 @@
       <c r="B91" t="s">
         <v>16</v>
       </c>
-      <c r="C91" s="3">
-        <v>1742327505408490</v>
+      <c r="C91" s="4">
+        <v>1.7423275054084899</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -1497,8 +1511,8 @@
       <c r="B92" t="s">
         <v>7</v>
       </c>
-      <c r="C92" s="3">
-        <v>1.70522033713781E+16</v>
+      <c r="C92" s="4">
+        <v>1.7052203371378101</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -1508,8 +1522,8 @@
       <c r="B93" t="s">
         <v>10</v>
       </c>
-      <c r="C93" s="3">
-        <v>1700179795483410</v>
+      <c r="C93" s="4">
+        <v>1.7001797954834099</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -1519,8 +1533,8 @@
       <c r="B94" t="s">
         <v>11</v>
       </c>
-      <c r="C94" s="3">
-        <v>1.69710485039184E+16</v>
+      <c r="C94" s="4">
+        <v>1.69710485039184</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -1530,8 +1544,8 @@
       <c r="B95" t="s">
         <v>15</v>
       </c>
-      <c r="C95" s="3">
-        <v>1.69624118958057E+16</v>
+      <c r="C95" s="4">
+        <v>1.69624118958057</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -1541,8 +1555,8 @@
       <c r="B96" t="s">
         <v>12</v>
       </c>
-      <c r="C96" s="3">
-        <v>1694104809233910</v>
+      <c r="C96" s="4">
+        <v>1.6941048092339099</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -1552,8 +1566,8 @@
       <c r="B97" t="s">
         <v>2</v>
       </c>
-      <c r="C97" s="3">
-        <v>1.69276310153215E+16</v>
+      <c r="C97" s="4">
+        <v>1.69276310153215</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -1563,8 +1577,8 @@
       <c r="B98" t="s">
         <v>6</v>
       </c>
-      <c r="C98" s="3">
-        <v>1692568549199970</v>
+      <c r="C98" s="4">
+        <v>1.69256854919997</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -1574,8 +1588,8 @@
       <c r="B99" t="s">
         <v>1</v>
       </c>
-      <c r="C99" s="3">
-        <v>1692436792344730</v>
+      <c r="C99" s="4">
+        <v>1.6924367923447301</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -1585,8 +1599,8 @@
       <c r="B100" t="s">
         <v>17</v>
       </c>
-      <c r="C100" s="3">
-        <v>1.69138384332405E+16</v>
+      <c r="C100" s="4">
+        <v>1.69138384332405</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -1596,8 +1610,8 @@
       <c r="B101" t="s">
         <v>13</v>
       </c>
-      <c r="C101" s="3">
-        <v>1690832465226890</v>
+      <c r="C101" s="4">
+        <v>1.69083246522689</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -1607,8 +1621,8 @@
       <c r="B102" t="s">
         <v>19</v>
       </c>
-      <c r="C102" s="3">
-        <v>1688474112744410</v>
+      <c r="C102" s="4">
+        <v>1.6884741127444101</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -1618,8 +1632,8 @@
       <c r="B103" t="s">
         <v>3</v>
       </c>
-      <c r="C103" s="3">
-        <v>1.68570490849385E+16</v>
+      <c r="C103" s="4">
+        <v>1.68570490849385</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -1629,8 +1643,8 @@
       <c r="B104" t="s">
         <v>0</v>
       </c>
-      <c r="C104" s="3">
-        <v>1685459762843120</v>
+      <c r="C104" s="4">
+        <v>1.68545976284312</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -1640,8 +1654,8 @@
       <c r="B105" t="s">
         <v>4</v>
       </c>
-      <c r="C105" s="3">
-        <v>1.68536336389156E+16</v>
+      <c r="C105" s="4">
+        <v>1.6853633638915599</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -1651,8 +1665,8 @@
       <c r="B106" t="s">
         <v>14</v>
       </c>
-      <c r="C106" s="3">
-        <v>1.6842912289947E+16</v>
+      <c r="C106" s="4">
+        <v>1.6842912289947001</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -1662,8 +1676,8 @@
       <c r="B107" t="s">
         <v>7</v>
       </c>
-      <c r="C107" s="3">
-        <v>2921790808789300</v>
+      <c r="C107" s="4">
+        <v>2.9217908087893001</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -1673,8 +1687,8 @@
       <c r="B108" t="s">
         <v>0</v>
       </c>
-      <c r="C108" s="3">
-        <v>2597680172628730</v>
+      <c r="C108" s="4">
+        <v>2.59768017262873</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -1684,8 +1698,8 @@
       <c r="B109" t="s">
         <v>11</v>
       </c>
-      <c r="C109" s="3">
-        <v>2.18817070475403E+16</v>
+      <c r="C109" s="4">
+        <v>2.1881707047540302</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -1695,8 +1709,8 @@
       <c r="B110" t="s">
         <v>19</v>
       </c>
-      <c r="C110" s="3">
-        <v>2.11098791826694E+16</v>
+      <c r="C110" s="4">
+        <v>2.11098791826694</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -1706,8 +1720,8 @@
       <c r="B111" t="s">
         <v>18</v>
       </c>
-      <c r="C111" s="3">
-        <v>2092557511608830</v>
+      <c r="C111" s="4">
+        <v>2.0925575116088302</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -1717,8 +1731,8 @@
       <c r="B112" t="s">
         <v>9</v>
       </c>
-      <c r="C112" s="3">
-        <v>1.69276310153215E+16</v>
+      <c r="C112" s="4">
+        <v>1.69276310153215</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -1728,8 +1742,8 @@
       <c r="B113" t="s">
         <v>1</v>
       </c>
-      <c r="C113" s="3">
-        <v>2923207976146770</v>
+      <c r="C113" s="4">
+        <v>2.9232079761467702</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -1739,8 +1753,8 @@
       <c r="B114" t="s">
         <v>2</v>
       </c>
-      <c r="C114" s="3">
-        <v>2921790808789300</v>
+      <c r="C114" s="4">
+        <v>2.9217908087893001</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -1750,8 +1764,8 @@
       <c r="B115" t="s">
         <v>11</v>
       </c>
-      <c r="C115" s="3">
-        <v>2616308305850640</v>
+      <c r="C115" s="4">
+        <v>2.61630830585064</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -1761,8 +1775,8 @@
       <c r="B116" t="s">
         <v>16</v>
       </c>
-      <c r="C116" s="3">
-        <v>260915987967025</v>
+      <c r="C116" s="4">
+        <v>2.6091598796702402</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -1772,8 +1786,8 @@
       <c r="B117" t="s">
         <v>6</v>
       </c>
-      <c r="C117" s="3">
-        <v>2286590236948410</v>
+      <c r="C117" s="4">
+        <v>2.2865902369484101</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -1783,8 +1797,8 @@
       <c r="B118" t="s">
         <v>17</v>
       </c>
-      <c r="C118" s="3">
-        <v>2278737125761410</v>
+      <c r="C118" s="4">
+        <v>2.2787371257614102</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -1794,8 +1808,8 @@
       <c r="B119" t="s">
         <v>5</v>
       </c>
-      <c r="C119" s="3">
-        <v>1.86372820157284E+16</v>
+      <c r="C119" s="4">
+        <v>1.86372820157284</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -1805,8 +1819,8 @@
       <c r="B120" t="s">
         <v>4</v>
       </c>
-      <c r="C120" s="3">
-        <v>1.85707166530735E+16</v>
+      <c r="C120" s="4">
+        <v>1.85707166530735</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -1816,8 +1830,8 @@
       <c r="B121" t="s">
         <v>0</v>
       </c>
-      <c r="C121" s="3">
-        <v>1771705453175350</v>
+      <c r="C121" s="4">
+        <v>1.77170545317535</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -1827,8 +1841,8 @@
       <c r="B122" t="s">
         <v>9</v>
       </c>
-      <c r="C122" s="3">
-        <v>1.70522033713781E+16</v>
+      <c r="C122" s="4">
+        <v>1.7052203371378101</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
@@ -1838,8 +1852,8 @@
       <c r="B123" t="s">
         <v>18</v>
       </c>
-      <c r="C123" s="3">
-        <v>1.69284761827952E+16</v>
+      <c r="C123" s="4">
+        <v>1.69284761827952</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
@@ -1849,8 +1863,8 @@
       <c r="B124" t="s">
         <v>19</v>
       </c>
-      <c r="C124" s="3">
-        <v>1690792476221010</v>
+      <c r="C124" s="4">
+        <v>1.69079247622101</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
@@ -1860,8 +1874,8 @@
       <c r="B125" t="s">
         <v>4</v>
       </c>
-      <c r="C125" s="3">
-        <v>2.861234948726E+16</v>
+      <c r="C125" s="4">
+        <v>2.861234948726</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
@@ -1871,8 +1885,8 @@
       <c r="B126" t="s">
         <v>5</v>
       </c>
-      <c r="C126" s="3">
-        <v>2.84302141578714E+16</v>
+      <c r="C126" s="4">
+        <v>2.8430214157871401</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
@@ -1882,8 +1896,8 @@
       <c r="B127" t="s">
         <v>19</v>
       </c>
-      <c r="C127" s="3">
-        <v>2656017136782450</v>
+      <c r="C127" s="4">
+        <v>2.6560171367824501</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
@@ -1893,8 +1907,8 @@
       <c r="B128" t="s">
         <v>18</v>
       </c>
-      <c r="C128" s="3">
-        <v>260134299002341</v>
+      <c r="C128" s="4">
+        <v>2.6013429900234</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
@@ -1904,8 +1918,8 @@
       <c r="B129" t="s">
         <v>11</v>
       </c>
-      <c r="C129" s="3">
-        <v>2.28910423902995E+16</v>
+      <c r="C129" s="4">
+        <v>2.2891042390299599</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
@@ -1915,8 +1929,8 @@
       <c r="B130" t="s">
         <v>9</v>
       </c>
-      <c r="C130" s="3">
-        <v>1.69624118958057E+16</v>
+      <c r="C130" s="4">
+        <v>1.69624118958057</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
@@ -1926,8 +1940,8 @@
       <c r="B131" t="s">
         <v>19</v>
       </c>
-      <c r="C131" s="3">
-        <v>2.48430918911104E+16</v>
+      <c r="C131" s="4">
+        <v>2.4843091891110398</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
@@ -1937,8 +1951,8 @@
       <c r="B132" t="s">
         <v>0</v>
       </c>
-      <c r="C132" s="3">
-        <v>2469419696189080</v>
+      <c r="C132" s="4">
+        <v>2.46941969618908</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
@@ -1948,8 +1962,8 @@
       <c r="B133" t="s">
         <v>18</v>
       </c>
-      <c r="C133" s="3">
-        <v>2.44144993186361E+16</v>
+      <c r="C133" s="4">
+        <v>2.4414499318636098</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
@@ -1959,8 +1973,8 @@
       <c r="B134" t="s">
         <v>11</v>
       </c>
-      <c r="C134" s="3">
-        <v>2.413547675853E+16</v>
+      <c r="C134" s="4">
+        <v>2.4135476758530001</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
@@ -1970,8 +1984,8 @@
       <c r="B135" t="s">
         <v>9</v>
       </c>
-      <c r="C135" s="3">
-        <v>1.68570490849385E+16</v>
+      <c r="C135" s="4">
+        <v>1.68570490849385</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
@@ -1981,8 +1995,8 @@
       <c r="B136" t="s">
         <v>5</v>
       </c>
-      <c r="C136" s="3">
-        <v>1.68141435344993E+16</v>
+      <c r="C136" s="4">
+        <v>1.68141435344993</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
@@ -1992,8 +2006,8 @@
       <c r="B137" t="s">
         <v>4</v>
       </c>
-      <c r="C137" s="3">
-        <v>1.67878330761273E+16</v>
+      <c r="C137" s="4">
+        <v>1.6787833076127301</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
@@ -2003,8 +2017,8 @@
       <c r="B138" t="s">
         <v>7</v>
       </c>
-      <c r="C138" s="3">
-        <v>260915987967025</v>
+      <c r="C138" s="4">
+        <v>2.6091598796702402</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
@@ -2014,8 +2028,8 @@
       <c r="B139" t="s">
         <v>11</v>
       </c>
-      <c r="C139" s="3">
-        <v>214990619808504</v>
+      <c r="C139" s="4">
+        <v>2.1499061980850298</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
@@ -2025,8 +2039,8 @@
       <c r="B140" t="s">
         <v>9</v>
       </c>
-      <c r="C140" s="3">
-        <v>1742327505408490</v>
+      <c r="C140" s="4">
+        <v>1.7423275054084899</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
@@ -2036,8 +2050,8 @@
       <c r="B141" t="s">
         <v>5</v>
       </c>
-      <c r="C141" s="3">
-        <v>1.73130908517924E+16</v>
+      <c r="C141" s="4">
+        <v>1.7313090851792401</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
@@ -2047,8 +2061,8 @@
       <c r="B142" t="s">
         <v>4</v>
       </c>
-      <c r="C142" s="3">
-        <v>1707418864496270</v>
+      <c r="C142" s="4">
+        <v>1.70741886449627</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
@@ -2058,8 +2072,8 @@
       <c r="B143" t="s">
         <v>1</v>
       </c>
-      <c r="C143" s="3">
-        <v>2.93523521438851E+16</v>
+      <c r="C143" s="4">
+        <v>2.9352352143885101</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
@@ -2069,8 +2083,8 @@
       <c r="B144" t="s">
         <v>15</v>
       </c>
-      <c r="C144" s="3">
-        <v>2.84302141578714E+16</v>
+      <c r="C144" s="4">
+        <v>2.8430214157871401</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
@@ -2080,8 +2094,8 @@
       <c r="B145" t="s">
         <v>9</v>
       </c>
-      <c r="C145" s="3">
-        <v>2.43021571881643E+16</v>
+      <c r="C145" s="4">
+        <v>2.4302157188164299</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
@@ -2091,8 +2105,8 @@
       <c r="B146" t="s">
         <v>0</v>
       </c>
-      <c r="C146" s="3">
-        <v>2.37778344190509E+16</v>
+      <c r="C146" s="4">
+        <v>2.3777834419050898</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
@@ -2102,8 +2116,8 @@
       <c r="B147" t="s">
         <v>18</v>
       </c>
-      <c r="C147" s="3">
-        <v>2.10500966253373E+16</v>
+      <c r="C147" s="4">
+        <v>2.10500966253373</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
@@ -2113,8 +2127,8 @@
       <c r="B148" t="s">
         <v>7</v>
       </c>
-      <c r="C148" s="3">
-        <v>1.86372820157284E+16</v>
+      <c r="C148" s="4">
+        <v>1.86372820157284</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
@@ -2124,8 +2138,8 @@
       <c r="B149" t="s">
         <v>8</v>
       </c>
-      <c r="C149" s="3">
-        <v>1.74877709099665E+16</v>
+      <c r="C149" s="4">
+        <v>1.74877709099665</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
@@ -2135,8 +2149,8 @@
       <c r="B150" t="s">
         <v>16</v>
       </c>
-      <c r="C150" s="3">
-        <v>1.73130908517924E+16</v>
+      <c r="C150" s="4">
+        <v>1.7313090851792401</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
@@ -2146,8 +2160,8 @@
       <c r="B151" t="s">
         <v>10</v>
       </c>
-      <c r="C151" s="3">
-        <v>1.69152904065201E+16</v>
+      <c r="C151" s="4">
+        <v>1.69152904065201</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
@@ -2157,8 +2171,8 @@
       <c r="B152" t="s">
         <v>11</v>
       </c>
-      <c r="C152" s="3">
-        <v>1690448028272840</v>
+      <c r="C152" s="4">
+        <v>1.69044802827284</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
@@ -2168,8 +2182,8 @@
       <c r="B153" t="s">
         <v>12</v>
       </c>
-      <c r="C153" s="3">
-        <v>1.6881049422915E+16</v>
+      <c r="C153" s="4">
+        <v>1.6881049422915</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
@@ -2179,8 +2193,8 @@
       <c r="B154" t="s">
         <v>6</v>
       </c>
-      <c r="C154" s="3">
-        <v>1.68656593144412E+16</v>
+      <c r="C154" s="4">
+        <v>1.6865659314441199</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
@@ -2190,8 +2204,8 @@
       <c r="B155" t="s">
         <v>13</v>
       </c>
-      <c r="C155" s="3">
-        <v>1.68566196135858E+16</v>
+      <c r="C155" s="4">
+        <v>1.6856619613585799</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
@@ -2201,8 +2215,8 @@
       <c r="B156" t="s">
         <v>17</v>
       </c>
-      <c r="C156" s="3">
-        <v>1685536223205350</v>
+      <c r="C156" s="4">
+        <v>1.6855362232053499</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
@@ -2212,8 +2226,8 @@
       <c r="B157" t="s">
         <v>19</v>
       </c>
-      <c r="C157" s="3">
-        <v>1.68456630103647E+16</v>
+      <c r="C157" s="4">
+        <v>1.68456630103647</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
@@ -2223,8 +2237,8 @@
       <c r="B158" t="s">
         <v>3</v>
       </c>
-      <c r="C158" s="3">
-        <v>1.68141435344993E+16</v>
+      <c r="C158" s="4">
+        <v>1.68141435344993</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
@@ -2234,8 +2248,8 @@
       <c r="B159" t="s">
         <v>14</v>
       </c>
-      <c r="C159" s="3">
-        <v>1.68089781568594E+16</v>
+      <c r="C159" s="4">
+        <v>1.68089781568594</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
@@ -2245,8 +2259,8 @@
       <c r="B160" t="s">
         <v>4</v>
       </c>
-      <c r="C160" s="3">
-        <v>2.95766267941654E+16</v>
+      <c r="C160" s="4">
+        <v>2.9576626794165399</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
@@ -2256,8 +2270,8 @@
       <c r="B161" t="s">
         <v>5</v>
       </c>
-      <c r="C161" s="3">
-        <v>2.93523521438851E+16</v>
+      <c r="C161" s="4">
+        <v>2.9352352143885101</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
@@ -2267,8 +2281,8 @@
       <c r="B162" t="s">
         <v>7</v>
       </c>
-      <c r="C162" s="3">
-        <v>2923207976146770</v>
+      <c r="C162" s="4">
+        <v>2.9232079761467702</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
@@ -2278,8 +2292,8 @@
       <c r="B163" t="s">
         <v>0</v>
       </c>
-      <c r="C163" s="3">
-        <v>2.69402037677742E+16</v>
+      <c r="C163" s="4">
+        <v>2.6940203767774298</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
@@ -2289,8 +2303,8 @@
       <c r="B164" t="s">
         <v>19</v>
       </c>
-      <c r="C164" s="3">
-        <v>2.32474927563521E+16</v>
+      <c r="C164" s="4">
+        <v>2.3247492756352099</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
@@ -2300,8 +2314,8 @@
       <c r="B165" t="s">
         <v>18</v>
       </c>
-      <c r="C165" s="3">
-        <v>2.29328205843498E+16</v>
+      <c r="C165" s="4">
+        <v>2.29328205843498</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
@@ -2311,8 +2325,8 @@
       <c r="B166" t="s">
         <v>11</v>
       </c>
-      <c r="C166" s="3">
-        <v>2196599519739470</v>
+      <c r="C166" s="4">
+        <v>2.1965995197394701</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
@@ -2322,8 +2336,8 @@
       <c r="B167" t="s">
         <v>9</v>
       </c>
-      <c r="C167" s="3">
-        <v>1692436792344730</v>
+      <c r="C167" s="4">
+        <v>1.6924367923447301</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
@@ -2333,8 +2347,8 @@
       <c r="B168" t="s">
         <v>9</v>
       </c>
-      <c r="C168" s="3">
-        <v>1700179795483410</v>
+      <c r="C168" s="4">
+        <v>1.7001797954834099</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
@@ -2344,8 +2358,8 @@
       <c r="B169" t="s">
         <v>5</v>
       </c>
-      <c r="C169" s="3">
-        <v>1.69152904065201E+16</v>
+      <c r="C169" s="4">
+        <v>1.69152904065201</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
@@ -2355,8 +2369,8 @@
       <c r="B170" t="s">
         <v>18</v>
       </c>
-      <c r="C170" s="3">
-        <v>1.68902751445241E+16</v>
+      <c r="C170" s="4">
+        <v>1.6890275144524101</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
@@ -2366,8 +2380,8 @@
       <c r="B171" t="s">
         <v>19</v>
       </c>
-      <c r="C171" s="3">
-        <v>1.68788194634332E+16</v>
+      <c r="C171" s="4">
+        <v>1.6878819463433199</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
@@ -2377,8 +2391,8 @@
       <c r="B172" t="s">
         <v>4</v>
       </c>
-      <c r="C172" s="3">
-        <v>1684578689698250</v>
+      <c r="C172" s="4">
+        <v>1.68457868969825</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
@@ -2388,8 +2402,8 @@
       <c r="B173" t="s">
         <v>0</v>
       </c>
-      <c r="C173" s="3">
-        <v>1.68395329860972E+16</v>
+      <c r="C173" s="4">
+        <v>1.6839532986097201</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
@@ -2399,8 +2413,8 @@
       <c r="B174" t="s">
         <v>6</v>
       </c>
-      <c r="C174" s="3">
-        <v>2.75438617362444E+16</v>
+      <c r="C174" s="4">
+        <v>2.7543861736244399</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
@@ -2410,8 +2424,8 @@
       <c r="B175" t="s">
         <v>17</v>
       </c>
-      <c r="C175" s="3">
-        <v>2.74351073603988E+16</v>
+      <c r="C175" s="4">
+        <v>2.7435107360398798</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
@@ -2421,8 +2435,8 @@
       <c r="B176" t="s">
         <v>11</v>
       </c>
-      <c r="C176" s="3">
-        <v>2484740990245300</v>
+      <c r="C176" s="4">
+        <v>2.4847409902452999</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
@@ -2432,8 +2446,8 @@
       <c r="B177" t="s">
         <v>9</v>
       </c>
-      <c r="C177" s="3">
-        <v>1.75580608424507E+16</v>
+      <c r="C177" s="4">
+        <v>1.75580608424507</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
@@ -2443,8 +2457,8 @@
       <c r="B178" t="s">
         <v>5</v>
       </c>
-      <c r="C178" s="3">
-        <v>1.74877709099665E+16</v>
+      <c r="C178" s="4">
+        <v>1.74877709099665</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
@@ -2454,8 +2468,8 @@
       <c r="B179" t="s">
         <v>18</v>
       </c>
-      <c r="C179" s="3">
-        <v>1.74610355312812E+16</v>
+      <c r="C179" s="4">
+        <v>1.7461035531281199</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
@@ -2465,8 +2479,8 @@
       <c r="B180" t="s">
         <v>0</v>
       </c>
-      <c r="C180" s="3">
-        <v>1.73205555486039E+16</v>
+      <c r="C180" s="4">
+        <v>1.73205555486039</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
@@ -2476,8 +2490,8 @@
       <c r="B181" t="s">
         <v>19</v>
       </c>
-      <c r="C181" s="3">
-        <v>1.72538787218592E+16</v>
+      <c r="C181" s="4">
+        <v>1.7253878721859199</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
@@ -2487,8 +2501,8 @@
       <c r="B182" t="s">
         <v>4</v>
       </c>
-      <c r="C182" s="3">
-        <v>1.7181573049434E+16</v>
+      <c r="C182" s="4">
+        <v>1.7181573049434</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
@@ -2498,8 +2512,8 @@
       <c r="B183" t="s">
         <v>15</v>
       </c>
-      <c r="C183" s="3">
-        <v>2656017136782450</v>
+      <c r="C183" s="4">
+        <v>2.6560171367824501</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
@@ -2509,8 +2523,8 @@
       <c r="B184" t="s">
         <v>3</v>
       </c>
-      <c r="C184" s="3">
-        <v>2.48430918911104E+16</v>
+      <c r="C184" s="4">
+        <v>2.4843091891110398</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
@@ -2520,8 +2534,8 @@
       <c r="B185" t="s">
         <v>1</v>
       </c>
-      <c r="C185" s="3">
-        <v>2.32474927563521E+16</v>
+      <c r="C185" s="4">
+        <v>2.3247492756352099</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
@@ -2531,8 +2545,8 @@
       <c r="B186" t="s">
         <v>2</v>
       </c>
-      <c r="C186" s="3">
-        <v>2.11098791826694E+16</v>
+      <c r="C186" s="4">
+        <v>2.11098791826694</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
@@ -2542,8 +2556,8 @@
       <c r="B187" t="s">
         <v>6</v>
       </c>
-      <c r="C187" s="3">
-        <v>2.0600694550104E+16</v>
+      <c r="C187" s="4">
+        <v>2.0600694550104</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
@@ -2553,8 +2567,8 @@
       <c r="B188" t="s">
         <v>8</v>
       </c>
-      <c r="C188" s="3">
-        <v>1.72538787218592E+16</v>
+      <c r="C188" s="4">
+        <v>1.7253878721859199</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
@@ -2564,8 +2578,8 @@
       <c r="B189" t="s">
         <v>7</v>
       </c>
-      <c r="C189" s="3">
-        <v>1690792476221010</v>
+      <c r="C189" s="4">
+        <v>1.69079247622101</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
@@ -2575,8 +2589,8 @@
       <c r="B190" t="s">
         <v>9</v>
       </c>
-      <c r="C190" s="3">
-        <v>1688474112744410</v>
+      <c r="C190" s="4">
+        <v>1.6884741127444101</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
@@ -2586,8 +2600,8 @@
       <c r="B191" t="s">
         <v>10</v>
       </c>
-      <c r="C191" s="3">
-        <v>1.68788194634332E+16</v>
+      <c r="C191" s="4">
+        <v>1.6878819463433199</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
@@ -2597,8 +2611,8 @@
       <c r="B192" t="s">
         <v>11</v>
       </c>
-      <c r="C192" s="3">
-        <v>1.68703327219465E+16</v>
+      <c r="C192" s="4">
+        <v>1.6870332721946499</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
@@ -2608,8 +2622,8 @@
       <c r="B193" t="s">
         <v>12</v>
       </c>
-      <c r="C193" s="3">
-        <v>1685344442868060</v>
+      <c r="C193" s="4">
+        <v>1.68534444286806</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
@@ -2619,8 +2633,8 @@
       <c r="B194" t="s">
         <v>5</v>
       </c>
-      <c r="C194" s="3">
-        <v>1.68456630103647E+16</v>
+      <c r="C194" s="4">
+        <v>1.68456630103647</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
@@ -2630,8 +2644,8 @@
       <c r="B195" t="s">
         <v>13</v>
       </c>
-      <c r="C195" s="3">
-        <v>168352987925093</v>
+      <c r="C195" s="4">
+        <v>1.6835298792509299</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
@@ -2641,8 +2655,8 @@
       <c r="B196" t="s">
         <v>4</v>
       </c>
-      <c r="C196" s="3">
-        <v>1.68090986136195E+16</v>
+      <c r="C196" s="4">
+        <v>1.68090986136195</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
@@ -2652,8 +2666,8 @@
       <c r="B197" t="s">
         <v>14</v>
       </c>
-      <c r="C197" s="3">
-        <v>1.67980988261053E+16</v>
+      <c r="C197" s="4">
+        <v>1.6798098826105301</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
@@ -2663,8 +2677,8 @@
       <c r="B198" t="s">
         <v>6</v>
       </c>
-      <c r="C198" s="3">
-        <v>2592838310912780</v>
+      <c r="C198" s="4">
+        <v>2.5928383109127799</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
@@ -2674,8 +2688,8 @@
       <c r="B199" t="s">
         <v>17</v>
       </c>
-      <c r="C199" s="3">
-        <v>2.58038902852308E+16</v>
+      <c r="C199" s="4">
+        <v>2.5803890285230802</v>
       </c>
       <c r="E199" s="1"/>
     </row>
@@ -2686,8 +2700,8 @@
       <c r="B200" t="s">
         <v>9</v>
       </c>
-      <c r="C200" s="3">
-        <v>1690832465226890</v>
+      <c r="C200" s="4">
+        <v>1.69083246522689</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
@@ -2697,8 +2711,8 @@
       <c r="B201" t="s">
         <v>5</v>
       </c>
-      <c r="C201" s="3">
-        <v>1.68566196135858E+16</v>
+      <c r="C201" s="4">
+        <v>1.6856619613585799</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
@@ -2708,8 +2722,8 @@
       <c r="B202" t="s">
         <v>18</v>
       </c>
-      <c r="C202" s="3">
-        <v>1684107791431590</v>
+      <c r="C202" s="4">
+        <v>1.6841077914315901</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
@@ -2719,8 +2733,8 @@
       <c r="B203" t="s">
         <v>19</v>
       </c>
-      <c r="C203" s="3">
-        <v>168352987925093</v>
+      <c r="C203" s="4">
+        <v>1.6835298792509299</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
@@ -2730,8 +2744,8 @@
       <c r="B204" t="s">
         <v>4</v>
       </c>
-      <c r="C204" s="3">
-        <v>1.68143257660378E+16</v>
+      <c r="C204" s="4">
+        <v>1.6814325766037801</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
@@ -2741,8 +2755,8 @@
       <c r="B205" t="s">
         <v>0</v>
       </c>
-      <c r="C205" s="3">
-        <v>1.68085413972208E+16</v>
+      <c r="C205" s="4">
+        <v>1.68085413972208</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
@@ -2752,8 +2766,8 @@
       <c r="B206" t="s">
         <v>8</v>
       </c>
-      <c r="C206" s="3">
-        <v>2.75438617362444E+16</v>
+      <c r="C206" s="4">
+        <v>2.7543861736244399</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
@@ -2763,8 +2777,8 @@
       <c r="B207" t="s">
         <v>14</v>
       </c>
-      <c r="C207" s="3">
-        <v>269582667556796</v>
+      <c r="C207" s="4">
+        <v>2.6958266755679601</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
@@ -2774,8 +2788,8 @@
       <c r="B208" t="s">
         <v>12</v>
       </c>
-      <c r="C208" s="3">
-        <v>2.62349025029971E+16</v>
+      <c r="C208" s="4">
+        <v>2.6234902502997102</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
@@ -2785,8 +2799,8 @@
       <c r="B209" t="s">
         <v>13</v>
       </c>
-      <c r="C209" s="3">
-        <v>2592838310912780</v>
+      <c r="C209" s="4">
+        <v>2.5928383109127799</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
@@ -2796,8 +2810,8 @@
       <c r="B210" t="s">
         <v>7</v>
       </c>
-      <c r="C210" s="3">
-        <v>2286590236948410</v>
+      <c r="C210" s="4">
+        <v>2.2865902369484101</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
@@ -2807,8 +2821,8 @@
       <c r="B211" t="s">
         <v>19</v>
       </c>
-      <c r="C211" s="3">
-        <v>2.0600694550104E+16</v>
+      <c r="C211" s="4">
+        <v>2.0600694550104</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
@@ -2818,8 +2832,8 @@
       <c r="B212" t="s">
         <v>0</v>
       </c>
-      <c r="C212" s="3">
-        <v>2.05241388507763E+16</v>
+      <c r="C212" s="4">
+        <v>2.0524138850776299</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
@@ -2829,8 +2843,8 @@
       <c r="B213" t="s">
         <v>18</v>
       </c>
-      <c r="C213" s="3">
-        <v>2.0446997306715E+16</v>
+      <c r="C213" s="4">
+        <v>2.0446997306714998</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
@@ -2840,8 +2854,8 @@
       <c r="B214" t="s">
         <v>11</v>
       </c>
-      <c r="C214" s="3">
-        <v>2.01117868118711E+16</v>
+      <c r="C214" s="4">
+        <v>2.01117868118711</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
@@ -2851,8 +2865,8 @@
       <c r="B215" t="s">
         <v>9</v>
       </c>
-      <c r="C215" s="3">
-        <v>1692568549199970</v>
+      <c r="C215" s="4">
+        <v>1.69256854919997</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
@@ -2862,8 +2876,8 @@
       <c r="B216" t="s">
         <v>5</v>
       </c>
-      <c r="C216" s="3">
-        <v>1.68656593144412E+16</v>
+      <c r="C216" s="4">
+        <v>1.6865659314441199</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
@@ -2873,8 +2887,8 @@
       <c r="B217" t="s">
         <v>4</v>
       </c>
-      <c r="C217" s="3">
-        <v>1.68188892900813E+16</v>
+      <c r="C217" s="4">
+        <v>1.68188892900813</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>